<commit_message>
still on Auth template
</commit_message>
<xml_diff>
--- a/php code libraries/Laravel DRY v1.xlsx
+++ b/php code libraries/Laravel DRY v1.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8340" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8340" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Laravel" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="LaravelGenerate" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="AutoLaravel v1" sheetId="6" r:id="rId3"/>
     <sheet name="laravelAuth v1" sheetId="7" r:id="rId4"/>
-    <sheet name="HTML template v1" sheetId="8" r:id="rId5"/>
+    <sheet name="Laravel mail v1" sheetId="10" r:id="rId5"/>
+    <sheet name="HTML template v1" sheetId="8" r:id="rId6"/>
+    <sheet name="error ptscreen" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="321">
   <si>
     <t>Fastest way of starting laravel 4 project:</t>
   </si>
@@ -788,9 +790,6 @@
     <t xml:space="preserve">laravel&gt;  </t>
   </si>
   <si>
-    <t>php artisan generate:migration create_users_table --fields="email:string,password:string"</t>
-  </si>
-  <si>
     <t>LARAVEL HTML TEMPLATE V1</t>
   </si>
   <si>
@@ -841,203 +840,447 @@
     <t>2. File structure must contain following content</t>
   </si>
   <si>
+    <t>(optional)</t>
+  </si>
+  <si>
+    <t>MAIN CONTENT HERE, USING TWITTER BOOTSTRAP RULES</t>
+  </si>
+  <si>
+    <t>3.  Modify header and footer files as desired. These are inside templates folder.</t>
+  </si>
+  <si>
+    <t>newuser</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Create:</t>
+  </si>
+  <si>
+    <t>LARAVEL AUTHENTICATION SYSTEM VERSION 1</t>
+  </si>
+  <si>
+    <t>1. Follow steps mentioned in AutoLaravel v1 up to the DB password line</t>
+  </si>
+  <si>
+    <t>Use the following standards</t>
+  </si>
+  <si>
+    <t>Table name</t>
+  </si>
+  <si>
+    <t>field names</t>
+  </si>
+  <si>
+    <t>Input id and name attributes (html form)</t>
+  </si>
+  <si>
+    <t>same of table field names</t>
+  </si>
+  <si>
+    <t>3. Create"user" controller</t>
+  </si>
+  <si>
+    <t>public function create() {</t>
+  </si>
+  <si>
+    <t>public function login() {</t>
+  </si>
+  <si>
+    <t>6. Open routes and create as default "login" action.  Indeed the next codes have all needed routes</t>
+  </si>
+  <si>
+    <t>Route::get('/','UserController@login');</t>
+  </si>
+  <si>
+    <t>Route::get('subscribe','UserController@create');</t>
+  </si>
+  <si>
+    <t>public function success() {</t>
+  </si>
+  <si>
+    <t>(delete default route)</t>
+  </si>
+  <si>
+    <t>2.  Use next command for creating users table and model:</t>
+  </si>
+  <si>
+    <t>php artisan generate:model User</t>
+  </si>
+  <si>
+    <t>Route::get('login','UserController@login');</t>
+  </si>
+  <si>
+    <t>Route::get('success',array('before'=&gt;'auth','uses'=&gt;'UserController@success'));</t>
+  </si>
+  <si>
+    <t>Route::get('adminuser',array('before'=&gt;'auth','uses'=&gt;'UserController@adminuser'));</t>
+  </si>
+  <si>
+    <t>… the user administration -adminuser- action</t>
+  </si>
+  <si>
+    <t>public function adminuser() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Return View::make('user.adminuser');</t>
+  </si>
+  <si>
+    <t>Basic login template</t>
+  </si>
+  <si>
+    <t>Copy - paste following folders as indicated</t>
+  </si>
+  <si>
+    <t>folder 'user' inside 'app/views'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "way/generators": "dev-master"</t>
+  </si>
+  <si>
+    <t>"laravel/framework": "4.0.*",</t>
+  </si>
+  <si>
+    <t>4. Open UserController and edit create action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt;with('title','subscribe');</t>
+  </si>
+  <si>
+    <t>Route::post('subscribe','UserController@suscription');</t>
+  </si>
+  <si>
+    <t>…  the login action</t>
+  </si>
+  <si>
+    <t>…  add the suscription action</t>
+  </si>
+  <si>
+    <t>public function suscription() {</t>
+  </si>
+  <si>
+    <t>//find if user exists. Give option to reset password</t>
+  </si>
+  <si>
+    <t>$count = User::where('email', '=', Input::get('new_email'))-&gt;count();</t>
+  </si>
+  <si>
+    <t>if ($count==0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Return View::make('user.newuser')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt;with('title','subscribe')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt;with('message','User already exists');</t>
+  </si>
+  <si>
+    <t>public function logout() {</t>
+  </si>
+  <si>
+    <t>… Add a "succesful login" -success- action</t>
+  </si>
+  <si>
+    <t>… Add a "logout" -success- action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Auth::logout();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    return View::make('user.logout')</t>
+  </si>
+  <si>
+    <t>Route::get('logout','UserController@logout');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -&gt;with('title','logged out');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Return View::make('user.success')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt;with('title','test loggedin page');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Return View::make('user.login')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt;with('title','Log in');</t>
+  </si>
+  <si>
+    <t>… verify login action</t>
+  </si>
+  <si>
+    <t>public function verifyuser(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        { return Redirect::to('success'); }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      return View::make('user.login')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -&gt;with('title','login')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -&gt;with('message','Wrong email or password'); }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   else { </t>
+  </si>
+  <si>
+    <t>esample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    $user=new User;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    $user-&gt;email=input::get('new_email');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    $user-&gt;password=Hash::make(input::get('new_password'));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    $user-&gt;save();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if (Auth::attempt(array( 'email' =&gt; input::get('new_email'), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else { return View::make('user.login'); }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        'password' =&gt; input::get('new_password') )))</t>
+  </si>
+  <si>
+    <t>Route::post('login','UserController@verifyuser');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if (Auth::attempt(array( 'email' =&gt; Input::get('email'), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        'password' =&gt; Input::get('password') )))</t>
+  </si>
+  <si>
+    <t>Next error is usual when POST route action (such as sending form) is not found</t>
+  </si>
+  <si>
+    <t>Solution: check if route::post('sameRouteDescribedOnPostURI'… and its controller action are properly set</t>
+  </si>
+  <si>
+    <t>Route::get('visible','UserController@visible');</t>
+  </si>
+  <si>
+    <t>…  add a 'any time visible' page, this is, regardless of logged in or out.</t>
+  </si>
+  <si>
+    <t>public function visible(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Return View::make('user.visible')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    -&gt;with('title','Visible');</t>
+  </si>
+  <si>
     <t>@extends('templates.base')</t>
   </si>
   <si>
-    <t xml:space="preserve">        @section('sidebar')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        @stop</t>
-  </si>
-  <si>
-    <t>(optional)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        @section('content')</t>
-  </si>
-  <si>
-    <t>MAIN CONTENT HERE, USING TWITTER BOOTSTRAP RULES</t>
-  </si>
-  <si>
-    <t>3.  Modify header and footer files as desired. These are inside templates folder.</t>
-  </si>
-  <si>
-    <t>newuser</t>
-  </si>
-  <si>
-    <t>Filename</t>
-  </si>
-  <si>
-    <t>Folder</t>
-  </si>
-  <si>
-    <t>Create:</t>
-  </si>
-  <si>
-    <t>LARAVEL AUTHENTICATION SYSTEM VERSION 1</t>
-  </si>
-  <si>
-    <t>1. Follow steps mentioned in AutoLaravel v1 up to the DB password line</t>
-  </si>
-  <si>
-    <t>Use the following standards</t>
-  </si>
-  <si>
-    <t>Table name</t>
-  </si>
-  <si>
-    <t>field names</t>
-  </si>
-  <si>
-    <t>Input id and name attributes (html form)</t>
-  </si>
-  <si>
-    <t>same of table field names</t>
-  </si>
-  <si>
-    <t>3. Create"user" controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Return View::make('user.newuser');</t>
-  </si>
-  <si>
-    <t>public function create() {</t>
-  </si>
-  <si>
-    <t>public function login() {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Return View::make('user.login');</t>
-  </si>
-  <si>
-    <t>6. Open routes and create as default "login" action.  Indeed the next codes have all needed routes</t>
-  </si>
-  <si>
-    <t>Route::get('/','UserController@login');</t>
-  </si>
-  <si>
-    <t>Route::get('subscribe','UserController@create');</t>
-  </si>
-  <si>
-    <t>… And add a "succesful login" -success- action</t>
-  </si>
-  <si>
-    <t>public function success() {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Return View::make('user.success');</t>
-  </si>
-  <si>
-    <t>(delete default route)</t>
-  </si>
-  <si>
-    <t>2.  Use next command for creating users table and model:</t>
-  </si>
-  <si>
-    <t>php artisan generate:model User</t>
-  </si>
-  <si>
-    <t>Route::get('login','UserController@login');</t>
-  </si>
-  <si>
-    <t>Route::get('success',array('before'=&gt;'auth','uses'=&gt;'UserController@success'));</t>
-  </si>
-  <si>
-    <t>Route::get('adminuser',array('before'=&gt;'auth','uses'=&gt;'UserController@adminuser'));</t>
-  </si>
-  <si>
-    <t>… the user administration -adminuser- action</t>
-  </si>
-  <si>
-    <t>public function adminuser() {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Return View::make('user.adminuser');</t>
-  </si>
-  <si>
-    <t>Basic login template</t>
-  </si>
-  <si>
-    <t>Copy - paste following folders as indicated</t>
-  </si>
-  <si>
-    <t>folder 'user' inside 'app/views'</t>
-  </si>
-  <si>
-    <t>csample</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "way/generators": "dev-master"</t>
-  </si>
-  <si>
-    <t>"laravel/framework": "4.0.*",</t>
-  </si>
-  <si>
-    <t>4. Open UserController and edit create action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    -&gt;with('title','subscribe');</t>
-  </si>
-  <si>
-    <t>Route::post('subscribe','UserController@suscription');</t>
-  </si>
-  <si>
-    <t>…  the login action</t>
-  </si>
-  <si>
-    <t>…  add the suscription action</t>
-  </si>
-  <si>
-    <t>public function suscription() {</t>
-  </si>
-  <si>
-    <t>//find if user exists. Give option to reset password</t>
-  </si>
-  <si>
-    <t>$count = User::where('email', '=', Input::get('new_email'))-&gt;count();</t>
-  </si>
-  <si>
-    <t>if ($count==0) {</t>
-  </si>
-  <si>
-    <t>$user=new User;</t>
-  </si>
-  <si>
-    <t>$user-&gt;email=input::get('new_email');</t>
-  </si>
-  <si>
-    <t>$user-&gt;password=Hash::make(input::get('new_password'));</t>
-  </si>
-  <si>
-    <t>$user-&gt;save();</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if (Auth::attempt(array( 'email' =&gt; input::get('new_email'), </t>
-  </si>
-  <si>
-    <t>'password' =&gt; input::get('new_password') )))</t>
-  </si>
-  <si>
-    <t>{ return Redirect::to('success'); }</t>
-  </si>
-  <si>
-    <t>else { return View::make('user.login'); }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Return View::make('user.newuser')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    -&gt;with('title','subscribe')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    -&gt;with('message','User already exists');</t>
+    <t xml:space="preserve"> @section('sidebar')</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @section('content')</t>
+  </si>
+  <si>
+    <t>from' =&gt; array('address' =&gt; 'no_reply@healmydisease.com', 'name' =&gt; 'Support'),</t>
+  </si>
+  <si>
+    <t>app/config/mail.php</t>
+  </si>
+  <si>
+    <t>'pretend' =&gt; true,</t>
+  </si>
+  <si>
+    <t>BE SURE TO SET FALSE WHEN WORKING ON REAL SERVER</t>
+  </si>
+  <si>
+    <t>host' =&gt; 'localhost',</t>
+  </si>
+  <si>
+    <t>resetkey</t>
+  </si>
+  <si>
+    <t>php artisan generate:migration create_users_table --fields="email:string,password:string,resetkey:string"</t>
+  </si>
+  <si>
+    <t>Since it was very traumatic, I will expose step by step mail function included in Laravel4</t>
+  </si>
+  <si>
+    <t>The first hard thing is to configurate email.php which is located at app/config/mail.php</t>
+  </si>
+  <si>
+    <t>'driver' =&gt; 'smtp',</t>
+  </si>
+  <si>
+    <t>'host' =&gt; 'whub32.webhostinghub.com',</t>
+  </si>
+  <si>
+    <t>'port' =&gt; 25,</t>
+  </si>
+  <si>
+    <t>'from' =&gt; array('address' =&gt; 'projectmanager@healmydisease.com', 'name' =&gt; 'Support'),</t>
+  </si>
+  <si>
+    <t>'encryption' =&gt; 'tls',</t>
+  </si>
+  <si>
+    <t>'username' =&gt; 'projectmanager@healmydisease.com',</t>
+  </si>
+  <si>
+    <t>'password' =&gt; 'laravel',</t>
+  </si>
+  <si>
+    <t>'sendmail' =&gt; '/usr/sbin/sendmail -bs',</t>
+  </si>
+  <si>
+    <t>'pretend' =&gt; false,</t>
+  </si>
+  <si>
+    <t>THE PREVIOUS PART IS MAYBE THE HARDEST COMPONENT OF LARAVEL MAIL.</t>
+  </si>
+  <si>
+    <t>The rest is relatively easy.</t>
+  </si>
+  <si>
+    <t>The previous code can be copy-pasted replacing all content of mail.php</t>
+  </si>
+  <si>
+    <t>Email syntax</t>
+  </si>
+  <si>
+    <t>Mail::send('view','data array','email recipient and subject closure');</t>
+  </si>
+  <si>
+    <t>View: works equal to View::make('xyz.abc') inside Views folder</t>
+  </si>
+  <si>
+    <t>$data (as data array): paired data array that can be called from email view as $variable</t>
+  </si>
+  <si>
+    <t>Email closure ($callback): closure that contains basic data, as recipient email, recipient</t>
+  </si>
+  <si>
+    <t>name and subject.</t>
+  </si>
+  <si>
+    <t>Mail::prepend();</t>
+  </si>
+  <si>
+    <t>Put this code above Mail::send to avoid sending from local host (and avoiding error messages).</t>
+  </si>
+  <si>
+    <t>On server comment this line.</t>
+  </si>
+  <si>
+    <t>When using "Mail::prepend" the log file generated at app/storage/logs (txt files)</t>
+  </si>
+  <si>
+    <t>informs each time a "send email" attempt is performed, with following syntax:</t>
+  </si>
+  <si>
+    <t>[2013-08-25 08:53:45] log.INFO: Pretending to mail message to: joaleto@yahoo.com [] []</t>
+  </si>
+  <si>
+    <t>Send email to an address entered to mail input field</t>
+  </si>
+  <si>
+    <t>As Input::get('field_x') can be stored in a $variable ($variable=Input::get('field'):</t>
+  </si>
+  <si>
+    <t>for unknown reasons it was not a good practice to send parameters with variable</t>
+  </si>
+  <si>
+    <t>instead of using the Input class itself.</t>
+  </si>
+  <si>
+    <t>});</t>
+  </si>
+  <si>
+    <t>//Mail::prepend()  /*uncomment on local, comment on hosted website*/</t>
+  </si>
+  <si>
+    <t>Template file: be aware that mail templates DO NOT LOAD EXTERNAL CSS FILES</t>
+  </si>
+  <si>
+    <t>Create a small &lt;style&gt;  …. &lt;/style&gt; segment inside the template in order to set</t>
+  </si>
+  <si>
+    <t>stylesheet.</t>
+  </si>
+  <si>
+    <t>Mail::send('templates.mail',array('User'=&gt;'Mr Someone'),function($message){</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Save email template as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>somefile.blade.php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and in the correct location use </t>
+    </r>
+  </si>
+  <si>
+    <t>{{$User}} (or any other variable) corresponding to the data array key.  It is obvious</t>
+  </si>
+  <si>
+    <t>to mention that the displayed information will be the value, not the key array.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    $message-&gt;to(Input::get('email'),'Mr. Someone')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '-&gt;subject('Requesting your portfolio');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THAT IS ALL.  MORE ATTRIBUTES CAN BE ADDED, SUCH AS CC AND CCO.  </t>
+  </si>
+  <si>
+    <t>Search at http://laravel.com/docs/mail for more information, as displayed instructions</t>
+  </si>
+  <si>
+    <t>on this spreadsheet are the basics for starting and resolving main needings.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1172,6 +1415,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1244,7 +1495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1273,6 +1524,9 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1317,6 +1571,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95250" y="685801"/>
+          <a:ext cx="6972300" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2210,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,7 +2588,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="D13" s="9"/>
     </row>
@@ -2296,7 +2598,7 @@
       </c>
       <c r="C14" s="23" t="str">
         <f>A1&amp;C13&amp;A2</f>
-        <v>composer create-project laravel/laravel csample --prefer-dist</v>
+        <v>composer create-project laravel/laravel esample --prefer-dist</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -2309,7 +2611,7 @@
       </c>
       <c r="C15" s="23" t="str">
         <f>"cd "&amp;C13</f>
-        <v>cd csample</v>
+        <v>cd esample</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2352,12 +2654,12 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="25" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="13" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D23" s="22"/>
     </row>
@@ -2419,7 +2721,7 @@
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="28" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2469,7 +2771,7 @@
       </c>
       <c r="M41" s="16" t="str">
         <f>IF(SUM(J46:K55)&gt;0,B2&amp;P55&amp;Q55&amp;B3,"")</f>
-        <v>--fields="email:string,password:string"</v>
+        <v>--fields="email:string,password:string,resetkey:string"</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
@@ -2607,8 +2909,12 @@
       <c r="B48" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
+      <c r="C48" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="F48" s="10" t="s">
         <v>116</v>
       </c>
@@ -2616,7 +2922,7 @@
       <c r="H48" s="9"/>
       <c r="J48" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="16">
         <f t="shared" si="1"/>
@@ -2627,7 +2933,7 @@
       </c>
       <c r="N48" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,resetkey:string</v>
       </c>
       <c r="O48" s="16" t="str">
         <f t="shared" si="3"/>
@@ -2635,7 +2941,7 @@
       </c>
       <c r="P48" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q48" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2674,7 +2980,7 @@
       </c>
       <c r="P49" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q49" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2713,7 +3019,7 @@
       </c>
       <c r="P50" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q50" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2752,7 +3058,7 @@
       </c>
       <c r="P51" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q51" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2791,7 +3097,7 @@
       </c>
       <c r="P52" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q52" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2830,7 +3136,7 @@
       </c>
       <c r="P53" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q53" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2869,7 +3175,7 @@
       </c>
       <c r="P54" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q54" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2908,7 +3214,7 @@
       </c>
       <c r="P55" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>email:string,password:string</v>
+        <v>email:string,password:string,resetkey:string</v>
       </c>
       <c r="Q55" s="16" t="str">
         <f t="shared" si="5"/>
@@ -2926,7 +3232,7 @@
       </c>
       <c r="C59" s="23" t="str">
         <f>A4&amp;A5&amp;A6&amp;D44&amp;B1&amp;M41</f>
-        <v>php artisan generate:migration create_users_table --fields="email:string,password:string"</v>
+        <v>php artisan generate:migration create_users_table --fields="email:string,password:string,resetkey:string"</v>
       </c>
       <c r="D59" s="23"/>
       <c r="E59" s="23"/>
@@ -2963,7 +3269,7 @@
         <v>149</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
@@ -2971,10 +3277,10 @@
         <v>150</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G65" s="22" t="str">
         <f>"app/views/"&amp;D66</f>
@@ -2990,7 +3296,7 @@
         <v>168</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G66" s="22" t="str">
         <f>D65&amp;".blade.php"</f>
@@ -3030,7 +3336,7 @@
         <v>160</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
@@ -3086,10 +3392,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I71"/>
+  <dimension ref="B3:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,63 +3403,63 @@
     <col min="1" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D9" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D11" s="10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>173</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>174</v>
+        <v>276</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -3161,8 +3467,10 @@
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>127</v>
       </c>
@@ -3174,12 +3482,12 @@
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>127</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -3188,7 +3496,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -3205,22 +3513,22 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="25" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="22" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="22" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -3230,254 +3538,415 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="C26" s="22"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" s="22" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="22" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="D28" s="22"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="22" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C30" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D35" s="22"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="D43" s="22"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" s="22"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C57" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D57" s="22"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D60" s="22"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="22" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="22"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C69" s="22"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="22"/>
+      <c r="C71" s="22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="22"/>
+      <c r="C72" s="27" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C73" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C74" s="22"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C75" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C76" s="22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C77" s="22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C78" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="22"/>
-      <c r="D31" s="22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="22"/>
-      <c r="D32" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="22"/>
-      <c r="D33" s="22" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="22"/>
-      <c r="D34" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="22"/>
-      <c r="E36" s="22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="22"/>
-      <c r="E37" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
+      <c r="F78" s="30"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C79" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="D41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C44" s="22"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C48" s="22"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="22" t="s">
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C80" s="22"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="22" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C52" s="22"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="22" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="22" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="22"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="22" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="22" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C60" s="22" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C61" s="22" t="s">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="22" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C63" s="22" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C64" s="22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="10" t="s">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="10" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="10" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="10" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C97" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C98" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C100" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="30" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C103" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C104" s="10" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3487,10 +3956,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D22"/>
+  <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,90 +3967,363 @@
     <col min="1" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="27" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="27" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="27" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>190</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="22" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="22" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="10" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="10" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="22" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="22" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add columns from cmd
</commit_message>
<xml_diff>
--- a/php code libraries/Laravel DRY v1.xlsx
+++ b/php code libraries/Laravel DRY v1.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8340" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8340" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Laravel" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="LaravelGenerate" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="LaravelGenerate" sheetId="5" r:id="rId2"/>
     <sheet name="FormGeneratorV1" sheetId="12" r:id="rId3"/>
     <sheet name="AutoLaravel v1" sheetId="6" r:id="rId4"/>
     <sheet name="laravelAuth v1" sheetId="7" r:id="rId5"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="400">
   <si>
     <t>Fastest way of starting laravel 4 project:</t>
   </si>
@@ -1255,21 +1255,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>newproject</t>
-  </si>
-  <si>
-    <t>add_new_project</t>
-  </si>
-  <si>
-    <t>new_prj_name</t>
-  </si>
-  <si>
-    <t>new_prj_goal</t>
-  </si>
-  <si>
-    <t>project_score</t>
-  </si>
-  <si>
     <t>TABLE RELATIONS METHODS V1</t>
   </si>
   <si>
@@ -1493,6 +1478,42 @@
   </si>
   <si>
     <t>&lt;?php }  ?&gt;</t>
+  </si>
+  <si>
+    <t>submit_task</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>4. Add column to table</t>
+  </si>
+  <si>
+    <t>ADDING COLUMNS TO TABLES</t>
+  </si>
+  <si>
+    <t>column name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>thetasks</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>php artisan generate:migration add_project_id_to_table_thetasks --fields="project_id:integer"</t>
+  </si>
+  <si>
+    <t>PENDING TO AUTOMATE WITH EXCEL CONCATENATIONS</t>
   </si>
 </sst>
 </file>
@@ -2669,7 +2690,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:XFD5"/>
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,91 +2700,91 @@
   <sheetData>
     <row r="1" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>282</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="48" t="s">
-        <v>355</v>
-      </c>
       <c r="C5" s="48" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="54" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
@@ -2773,7 +2794,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="54" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="54"/>
@@ -2783,17 +2804,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -2808,7 +2829,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -2819,7 +2840,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="50" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
@@ -2836,7 +2857,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="50" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -2853,7 +2874,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="51" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
@@ -2875,25 +2896,25 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>304</v>
@@ -2910,7 +2931,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>303</v>
@@ -2921,10 +2942,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="16" t="str">
@@ -2938,7 +2959,7 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>168</v>
@@ -2949,34 +2970,34 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D42" s="22" t="str">
         <f>F34&amp;"_id"</f>
         <v>project_id</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -3004,7 +3025,7 @@
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -3032,25 +3053,25 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" s="22" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D59" s="22" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -3059,7 +3080,7 @@
         <v>$project=Project::all();</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -3068,7 +3089,7 @@
         <v>foreach ($project as $value){</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -3077,7 +3098,7 @@
         <v xml:space="preserve">     $row=Project::find($value-&gt;id);</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -3086,7 +3107,7 @@
         <v xml:space="preserve">     $owner=$value-&gt;p_owner;</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -3095,22 +3116,22 @@
         <v xml:space="preserve">     $allowed=$row-&gt;projectpermission;</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D65" s="22" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D67" s="22" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
@@ -3121,82 +3142,82 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D69" s="10" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D70" s="10" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D71" s="10" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D72" s="10" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D73" s="10" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D74" s="10" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D75" s="22" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D76" s="22" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D77" s="10" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D78" s="10" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D79" s="10" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D80" s="10" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="10" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="10" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="22" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="22" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -3206,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I49"/>
+  <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,10 +3502,29 @@
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>86</v>
       </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3496,8 +3536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3604,16 +3644,16 @@
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="34" t="str">
         <f>IF('AutoLaravel v1'!C46&lt;&gt;"",'AutoLaravel v1'!C46,"")</f>
-        <v>new_prj_name</v>
+        <v>task</v>
       </c>
       <c r="C17" s="35" t="str">
         <f>IF(B17="","",'AutoLaravel v1'!$D$44&amp;"_"&amp;B17)</f>
-        <v>projects_new_prj_name</v>
+        <v>projects_task</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="35" t="str">
         <f>IF(B17="","",C17&amp;$A$1)</f>
-        <v>projects_new_prj_name_mssg</v>
+        <v>projects_task_mssg</v>
       </c>
       <c r="F17" s="36"/>
       <c r="H17" s="34" t="str">
@@ -3632,7 +3672,7 @@
       <c r="L17" s="36"/>
       <c r="N17" s="42" t="str">
         <f>B17</f>
-        <v>new_prj_name</v>
+        <v>task</v>
       </c>
       <c r="O17" s="43" t="str">
         <f>IF(H17&lt;&gt;"",",","")&amp;H17</f>
@@ -3642,16 +3682,16 @@
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="str">
         <f>IF('AutoLaravel v1'!C47&lt;&gt;"",'AutoLaravel v1'!C47,"")</f>
-        <v>new_prj_goal</v>
+        <v>project</v>
       </c>
       <c r="C18" s="33" t="str">
         <f>IF(B18="","",'AutoLaravel v1'!$D$44&amp;"_"&amp;B18)</f>
-        <v>projects_new_prj_goal</v>
+        <v>projects_project</v>
       </c>
       <c r="D18" s="33"/>
       <c r="E18" s="33" t="str">
         <f t="shared" ref="E18:E26" si="1">IF(B18="","",C18&amp;$A$1)</f>
-        <v>projects_new_prj_goal_mssg</v>
+        <v>projects_project_mssg</v>
       </c>
       <c r="F18" s="38"/>
       <c r="H18" s="37" t="str">
@@ -3670,7 +3710,7 @@
       <c r="L18" s="38"/>
       <c r="N18" s="44" t="str">
         <f>IF(B18&lt;&gt;"",",","")&amp;B18</f>
-        <v>,new_prj_goal</v>
+        <v>,project</v>
       </c>
       <c r="O18" s="45" t="str">
         <f t="shared" ref="O18:O26" si="2">IF(H18&lt;&gt;"",",","")&amp;H18</f>
@@ -3680,16 +3720,16 @@
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="str">
         <f>IF('AutoLaravel v1'!C48&lt;&gt;"",'AutoLaravel v1'!C48,"")</f>
-        <v>project_score</v>
+        <v>score</v>
       </c>
       <c r="C19" s="33" t="str">
         <f>IF(B19="","",'AutoLaravel v1'!$D$44&amp;"_"&amp;B19)</f>
-        <v>projects_project_score</v>
+        <v>projects_score</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>projects_project_score_mssg</v>
+        <v>projects_score_mssg</v>
       </c>
       <c r="F19" s="38"/>
       <c r="H19" s="37" t="str">
@@ -3708,7 +3748,7 @@
       <c r="L19" s="38"/>
       <c r="N19" s="44" t="str">
         <f t="shared" ref="N19:N26" si="3">IF(B19&lt;&gt;"",",","")&amp;B19</f>
-        <v>,project_score</v>
+        <v>,score</v>
       </c>
       <c r="O19" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3983,7 +4023,7 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="52" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C29" s="52"/>
       <c r="D29" s="52"/>
@@ -3993,7 +4033,7 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="52" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C30" s="52"/>
       <c r="D30" s="52"/>
@@ -4003,7 +4043,7 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="52" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C31" s="52"/>
       <c r="D31" s="52"/>
@@ -4013,7 +4053,7 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="52" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C32" s="52"/>
       <c r="D32" s="52"/>
@@ -4031,11 +4071,11 @@
         <v>275</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="E35" s="16" t="str">
         <f>UPPER(LEFT(D35,1))&amp;RIGHT(D35,LEN(D35)-1)</f>
-        <v>Newproject</v>
+        <v>Addtask</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -4055,7 +4095,7 @@
         <v>301</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>314</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -4064,7 +4104,7 @@
       </c>
       <c r="D38" s="32" t="str">
         <f>D36&amp;"/"&amp;D35</f>
-        <v>logged/newproject</v>
+        <v>logged/addtask</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -4075,13 +4115,13 @@
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="str">
         <f>$A$5&amp;D37&amp;A6</f>
-        <v>$('#add_new_project').click(function() {</v>
+        <v>$('#submit_task').click(function() {</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="32" t="str">
         <f>IF(B17="","",$A$2&amp;B17&amp;$A$3&amp;B17&amp;$A$4)&amp;IF(B18="","",$A$2&amp;B18&amp;$A$3&amp;B18&amp;$A$4)</f>
-        <v>var new_prj_name=$('#new_prj_name').val();var new_prj_goal=$('#new_prj_goal').val();</v>
+        <v>var task=$('#task').val();var project=$('#project').val();</v>
       </c>
       <c r="C41" s="32"/>
       <c r="D41" s="32"/>
@@ -4091,7 +4131,7 @@
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="32" t="str">
         <f>IF(B19="","",$A$2&amp;B19&amp;$A$3&amp;B19&amp;$A$4)&amp;IF(B20="","",$A$2&amp;B20&amp;$A$3&amp;B20&amp;$A$4)</f>
-        <v>var project_score=$('#project_score').val();</v>
+        <v>var score=$('#score').val();</v>
       </c>
       <c r="C42" s="32"/>
       <c r="D42" s="32"/>
@@ -4186,7 +4226,7 @@
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="23" t="str">
         <f>N17&amp;IF(B17&lt;&gt;"",":","")&amp;B17&amp;N18&amp;IF(B18&lt;&gt;"",":","")&amp;B18&amp;N19&amp;IF(B19&lt;&gt;"",":","")&amp;B19&amp;N20&amp;IF(B20&lt;&gt;"",":","")&amp;B20</f>
-        <v>new_prj_name:new_prj_name,new_prj_goal:new_prj_goal,project_score:project_score</v>
+        <v>task:task,project:project,score:score</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
@@ -4227,7 +4267,7 @@
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="str">
         <f>B1&amp;D38&amp;B2</f>
-        <v>var route='logged/newproject';</v>
+        <v>var route='logged/addtask';</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -4257,7 +4297,7 @@
       </c>
       <c r="D65" s="32" t="str">
         <f>"public function post"&amp;E35&amp;"() {}"</f>
-        <v>public function postNewproject() {}</v>
+        <v>public function postAddtask() {}</v>
       </c>
       <c r="E65" s="32"/>
       <c r="F65" s="32"/>
@@ -4265,19 +4305,19 @@
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="str">
         <f>"$"&amp;B17&amp;"=Input::get('"&amp;B17&amp;"');"</f>
-        <v>$new_prj_name=Input::get('new_prj_name');</v>
+        <v>$task=Input::get('task');</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="str">
         <f t="shared" ref="B67:B68" si="6">"$"&amp;B18&amp;"=Input::get('"&amp;B18&amp;"');"</f>
-        <v>$new_prj_goal=Input::get('new_prj_goal');</v>
+        <v>$project=Input::get('project');</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>$project_score=Input::get('project_score');</v>
+        <v>$score=Input::get('score');</v>
       </c>
     </row>
   </sheetData>
@@ -4288,10 +4328,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4549,7 +4589,7 @@
       </c>
       <c r="M41" s="16" t="str">
         <f>IF(SUM(J46:K55)&gt;0,B2&amp;P55&amp;Q55&amp;B3,"")</f>
-        <v>--fields="new_prj_name:string,new_prj_goal:string"</v>
+        <v>--fields="task:string,project:string,score:string"</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
@@ -4602,7 +4642,7 @@
         <v>103</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>315</v>
+        <v>389</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>134</v>
@@ -4625,7 +4665,7 @@
       </c>
       <c r="N46" s="16" t="str">
         <f>IF(AND(C46&lt;&gt;"",D46&lt;&gt;""),IF(N45="concatenator1","",",")&amp;C46&amp;":"&amp;D46,"")</f>
-        <v>new_prj_name:string</v>
+        <v>task:string</v>
       </c>
       <c r="O46" s="16" t="str">
         <f>IF(AND(G46&lt;&gt;"",H46&lt;&gt;""),","&amp;G46&amp;":"&amp;H46,"")</f>
@@ -4633,7 +4673,7 @@
       </c>
       <c r="P46" s="16" t="str">
         <f>P45&amp;N46</f>
-        <v>new_prj_name:string</v>
+        <v>task:string</v>
       </c>
       <c r="Q46" s="16" t="str">
         <f>Q45&amp;O46</f>
@@ -4645,7 +4685,7 @@
         <v>104</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>316</v>
+        <v>390</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>134</v>
@@ -4668,7 +4708,7 @@
       </c>
       <c r="N47" s="16" t="str">
         <f t="shared" ref="N47:N55" si="2">IF(AND(C47&lt;&gt;"",D47&lt;&gt;""),IF(N46="concatenator1","",",")&amp;C47&amp;":"&amp;D47,"")</f>
-        <v>,new_prj_goal:string</v>
+        <v>,project:string</v>
       </c>
       <c r="O47" s="16" t="str">
         <f t="shared" ref="O47:O55" si="3">IF(AND(G47&lt;&gt;"",H47&lt;&gt;""),","&amp;G47&amp;":"&amp;H47,"")</f>
@@ -4676,7 +4716,7 @@
       </c>
       <c r="P47" s="16" t="str">
         <f t="shared" ref="P47:P55" si="4">P46&amp;N47</f>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string</v>
       </c>
       <c r="Q47" s="16" t="str">
         <f t="shared" ref="Q47:Q55" si="5">Q46&amp;O47</f>
@@ -4688,9 +4728,11 @@
         <v>105</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="D48" s="9"/>
+        <v>391</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F48" s="10" t="s">
         <v>115</v>
       </c>
@@ -4709,7 +4751,7 @@
       </c>
       <c r="N48" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,score:string</v>
       </c>
       <c r="O48" s="16" t="str">
         <f t="shared" si="3"/>
@@ -4717,7 +4759,7 @@
       </c>
       <c r="P48" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q48" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4756,7 +4798,7 @@
       </c>
       <c r="P49" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q49" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4795,7 +4837,7 @@
       </c>
       <c r="P50" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q50" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4834,7 +4876,7 @@
       </c>
       <c r="P51" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q51" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4873,7 +4915,7 @@
       </c>
       <c r="P52" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q52" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4912,7 +4954,7 @@
       </c>
       <c r="P53" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q53" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4951,7 +4993,7 @@
       </c>
       <c r="P54" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q54" s="16" t="str">
         <f t="shared" si="5"/>
@@ -4990,7 +5032,7 @@
       </c>
       <c r="P55" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>new_prj_name:string,new_prj_goal:string</v>
+        <v>task:string,project:string,score:string</v>
       </c>
       <c r="Q55" s="16" t="str">
         <f t="shared" si="5"/>
@@ -5008,7 +5050,7 @@
       </c>
       <c r="C59" s="23" t="str">
         <f>A4&amp;A5&amp;A6&amp;D44&amp;B1&amp;M41</f>
-        <v>php artisan generate:migration create_projects_table --fields="new_prj_name:string,new_prj_goal:string"</v>
+        <v>php artisan generate:migration create_projects_table --fields="task:string,project:string,score:string"</v>
       </c>
       <c r="D59" s="23"/>
       <c r="E59" s="23"/>
@@ -5154,6 +5196,54 @@
         <f>"Route::get('"&amp;D65&amp;"','"&amp;G67&amp;"@"&amp;D69&amp;"');"</f>
         <v>Route::get('newuser','LoggedController@newuser');</v>
       </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C82" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+      <c r="K82" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5610,7 +5700,7 @@
   <dimension ref="B3:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5740,7 +5830,7 @@
         <v>283</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -5748,7 +5838,7 @@
         <v>274</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5839,7 +5929,7 @@
         <v>alejo/addtask</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First email template html
</commit_message>
<xml_diff>
--- a/php code libraries/Laravel DRY v1.xlsx
+++ b/php code libraries/Laravel DRY v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8340" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8340" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Laravel" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,8 +21,7 @@
     <sheet name="Laravel mail v1" sheetId="10" r:id="rId7"/>
     <sheet name="Controller generator" sheetId="11" r:id="rId8"/>
     <sheet name="table relations v1" sheetId="13" r:id="rId9"/>
-    <sheet name="Relations2" sheetId="14" r:id="rId10"/>
-    <sheet name="error ptscreen" sheetId="9" r:id="rId11"/>
+    <sheet name="error ptscreen" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="474">
   <si>
     <t>Fastest way of starting laravel 4 project:</t>
   </si>
@@ -973,9 +972,6 @@
     <t>name and subject.</t>
   </si>
   <si>
-    <t>Mail::prepend();</t>
-  </si>
-  <si>
     <t>Put this code above Mail::send to avoid sending from local host (and avoiding error messages).</t>
   </si>
   <si>
@@ -1106,15 +1102,9 @@
     <t>URI prefix</t>
   </si>
   <si>
-    <t>alejo</t>
-  </si>
-  <si>
     <t>Controller name</t>
   </si>
   <si>
-    <t>alex</t>
-  </si>
-  <si>
     <t>Route</t>
   </si>
   <si>
@@ -1463,12 +1453,6 @@
     <t>project_id</t>
   </si>
   <si>
-    <t>php artisan generate:migration add_project_id_to_table_thetasks --fields="project_id:integer"</t>
-  </si>
-  <si>
-    <t>PENDING TO AUTOMATE WITH EXCEL CONCATENATIONS</t>
-  </si>
-  <si>
     <t>var base=$('#base').html();</t>
   </si>
   <si>
@@ -1499,15 +1483,6 @@
     <t>//saving data</t>
   </si>
   <si>
-    <t>METHOD FOR RETRIEVING DATA FROM TABLE WITH PERMISSIONS STABLISHED IN TWO OTHER TABLES</t>
-  </si>
-  <si>
-    <t>Main table name</t>
-  </si>
-  <si>
-    <t>tasks</t>
-  </si>
-  <si>
     <t>cd ../../wamp/www/practice</t>
   </si>
   <si>
@@ -1562,15 +1537,6 @@
     <t>periods</t>
   </si>
   <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>minutes</t>
-  </si>
-  <si>
-    <t>seconds</t>
-  </si>
-  <si>
     <t>METHOD FOR COUNTING ITEMS FROM A TABLE WHEN CONDITION IS IN ANOTHER TABLE</t>
   </si>
   <si>
@@ -1716,6 +1682,60 @@
   </si>
   <si>
     <t xml:space="preserve">           example {{$value-&gt;score}} (if "name" is a column of desired main table) &lt;br&gt;</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>Inside html template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div&gt;Some message {{$User}}, please be careful with...&lt;/div&gt; </t>
+  </si>
+  <si>
+    <t>Mail::pretend();</t>
+  </si>
+  <si>
+    <t>junks</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>adopter</t>
+  </si>
+  <si>
+    <t>evidence</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <t>php artisan generate:migration add_</t>
+  </si>
+  <si>
+    <t>_to_</t>
+  </si>
+  <si>
+    <t>taskController</t>
   </si>
 </sst>
 </file>
@@ -2900,37 +2920,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="11.42578125" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>396</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3242,7 +3231,7 @@
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -3269,8 +3258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3278,167 +3267,167 @@
     <col min="1" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>388</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="B3" s="19" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="B4" s="19" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>295</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>297</v>
-      </c>
       <c r="B6" s="19" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="34" t="str">
         <f>IF('AutoLaravel v1'!C47&lt;&gt;"",'AutoLaravel v1'!C47,"")</f>
-        <v>hours</v>
+        <v>task</v>
       </c>
       <c r="C17" s="35" t="str">
         <f>IF(B17="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B17)</f>
-        <v>periods_hours</v>
+        <v>junks_task</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="35" t="str">
         <f>IF(B17="","",C17&amp;$A$1)</f>
-        <v>periods_hours_mssg</v>
+        <v>junks_task_mssg</v>
       </c>
       <c r="F17" s="36"/>
       <c r="H17" s="37" t="str">
         <f>IF('AutoLaravel v1'!G47&lt;&gt;"",'AutoLaravel v1'!G47,"")</f>
-        <v/>
+        <v>comments</v>
       </c>
       <c r="I17" s="35" t="str">
         <f>IF(H17&lt;&gt;"",'AutoLaravel v1'!$D$45&amp;"_"&amp;H17,"")</f>
-        <v/>
+        <v>junks_comments</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35" t="str">
         <f t="shared" ref="K17:K26" si="0">I17&amp;$A$1</f>
-        <v>_mssg</v>
+        <v>junks_comments_mssg</v>
       </c>
       <c r="L17" s="36"/>
       <c r="N17" s="42" t="str">
         <f>B17</f>
-        <v>hours</v>
+        <v>task</v>
       </c>
       <c r="O17" s="43" t="str">
         <f>IF(H17&lt;&gt;"",",","")&amp;H17</f>
-        <v/>
+        <v>,comments</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="str">
         <f>IF('AutoLaravel v1'!C48&lt;&gt;"",'AutoLaravel v1'!C48,"")</f>
-        <v>minutes</v>
+        <v>project</v>
       </c>
       <c r="C18" s="33" t="str">
         <f>IF(B18="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B18)</f>
-        <v>periods_minutes</v>
+        <v>junks_project</v>
       </c>
       <c r="D18" s="33"/>
       <c r="E18" s="33" t="str">
         <f t="shared" ref="E18:E26" si="1">IF(B18="","",C18&amp;$A$1)</f>
-        <v>periods_minutes_mssg</v>
+        <v>junks_project_mssg</v>
       </c>
       <c r="F18" s="38"/>
       <c r="H18" s="37" t="str">
@@ -3457,7 +3446,7 @@
       <c r="L18" s="38"/>
       <c r="N18" s="44" t="str">
         <f>IF(B18&lt;&gt;"",",","")&amp;B18</f>
-        <v>,minutes</v>
+        <v>,project</v>
       </c>
       <c r="O18" s="45" t="str">
         <f t="shared" ref="O18:O26" si="2">IF(H18&lt;&gt;"",",","")&amp;H18</f>
@@ -3467,16 +3456,16 @@
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="str">
         <f>IF('AutoLaravel v1'!C49&lt;&gt;"",'AutoLaravel v1'!C49,"")</f>
-        <v>seconds</v>
+        <v>stage</v>
       </c>
       <c r="C19" s="33" t="str">
         <f>IF(B19="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B19)</f>
-        <v>periods_seconds</v>
+        <v>junks_stage</v>
       </c>
       <c r="D19" s="33"/>
       <c r="E19" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>periods_seconds_mssg</v>
+        <v>junks_stage_mssg</v>
       </c>
       <c r="F19" s="38"/>
       <c r="H19" s="37" t="str">
@@ -3495,7 +3484,7 @@
       <c r="L19" s="38"/>
       <c r="N19" s="44" t="str">
         <f t="shared" ref="N19:N26" si="3">IF(B19&lt;&gt;"",",","")&amp;B19</f>
-        <v>,seconds</v>
+        <v>,stage</v>
       </c>
       <c r="O19" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3505,16 +3494,16 @@
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="str">
         <f>IF('AutoLaravel v1'!C50&lt;&gt;"",'AutoLaravel v1'!C50,"")</f>
-        <v/>
+        <v>parent</v>
       </c>
       <c r="C20" s="33" t="str">
         <f>IF(B20="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B20)</f>
-        <v/>
+        <v>junks_parent</v>
       </c>
       <c r="D20" s="33"/>
       <c r="E20" s="33" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_parent_mssg</v>
       </c>
       <c r="F20" s="38"/>
       <c r="H20" s="37" t="str">
@@ -3533,7 +3522,7 @@
       <c r="L20" s="38"/>
       <c r="N20" s="44" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,parent</v>
       </c>
       <c r="O20" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3543,16 +3532,16 @@
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="str">
         <f>IF('AutoLaravel v1'!C51&lt;&gt;"",'AutoLaravel v1'!C51,"")</f>
-        <v/>
+        <v>score</v>
       </c>
       <c r="C21" s="33" t="str">
         <f>IF(B21="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B21)</f>
-        <v/>
+        <v>junks_score</v>
       </c>
       <c r="D21" s="33"/>
       <c r="E21" s="33" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_score_mssg</v>
       </c>
       <c r="F21" s="38"/>
       <c r="H21" s="37" t="str">
@@ -3571,7 +3560,7 @@
       <c r="L21" s="38"/>
       <c r="N21" s="44" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,score</v>
       </c>
       <c r="O21" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3581,16 +3570,16 @@
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="str">
         <f>IF('AutoLaravel v1'!C52&lt;&gt;"",'AutoLaravel v1'!C52,"")</f>
-        <v/>
+        <v>creator</v>
       </c>
       <c r="C22" s="33" t="str">
         <f>IF(B22="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B22)</f>
-        <v/>
+        <v>junks_creator</v>
       </c>
       <c r="D22" s="33"/>
       <c r="E22" s="33" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_creator_mssg</v>
       </c>
       <c r="F22" s="38"/>
       <c r="H22" s="37" t="str">
@@ -3609,7 +3598,7 @@
       <c r="L22" s="38"/>
       <c r="N22" s="44" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,creator</v>
       </c>
       <c r="O22" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3619,16 +3608,16 @@
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="str">
         <f>IF('AutoLaravel v1'!C53&lt;&gt;"",'AutoLaravel v1'!C53,"")</f>
-        <v/>
+        <v>adopter</v>
       </c>
       <c r="C23" s="33" t="str">
         <f>IF(B23="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B23)</f>
-        <v/>
+        <v>junks_adopter</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="33" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_adopter_mssg</v>
       </c>
       <c r="F23" s="38"/>
       <c r="H23" s="37" t="str">
@@ -3647,7 +3636,7 @@
       <c r="L23" s="38"/>
       <c r="N23" s="44" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,adopter</v>
       </c>
       <c r="O23" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3657,16 +3646,16 @@
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="str">
         <f>IF('AutoLaravel v1'!C54&lt;&gt;"",'AutoLaravel v1'!C54,"")</f>
-        <v/>
+        <v>evidence</v>
       </c>
       <c r="C24" s="33" t="str">
         <f>IF(B24="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B24)</f>
-        <v/>
+        <v>junks_evidence</v>
       </c>
       <c r="D24" s="33"/>
       <c r="E24" s="33" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_evidence_mssg</v>
       </c>
       <c r="F24" s="38"/>
       <c r="H24" s="37" t="str">
@@ -3685,7 +3674,7 @@
       <c r="L24" s="38"/>
       <c r="N24" s="44" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,evidence</v>
       </c>
       <c r="O24" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3695,16 +3684,16 @@
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="str">
         <f>IF('AutoLaravel v1'!C55&lt;&gt;"",'AutoLaravel v1'!C55,"")</f>
-        <v/>
+        <v>reason</v>
       </c>
       <c r="C25" s="33" t="str">
         <f>IF(B25="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B25)</f>
-        <v/>
+        <v>junks_reason</v>
       </c>
       <c r="D25" s="33"/>
       <c r="E25" s="33" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_reason_mssg</v>
       </c>
       <c r="F25" s="38"/>
       <c r="H25" s="37" t="str">
@@ -3723,7 +3712,7 @@
       <c r="L25" s="38"/>
       <c r="N25" s="44" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,reason</v>
       </c>
       <c r="O25" s="45" t="str">
         <f t="shared" si="2"/>
@@ -3733,16 +3722,16 @@
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="39" t="str">
         <f>IF('AutoLaravel v1'!C56&lt;&gt;"",'AutoLaravel v1'!C56,"")</f>
-        <v/>
+        <v>output</v>
       </c>
       <c r="C26" s="40" t="str">
         <f>IF(B26="","",'AutoLaravel v1'!$D$45&amp;"_"&amp;B26)</f>
-        <v/>
+        <v>junks_output</v>
       </c>
       <c r="D26" s="40"/>
       <c r="E26" s="40" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>junks_output_mssg</v>
       </c>
       <c r="F26" s="41"/>
       <c r="H26" s="39" t="str">
@@ -3761,7 +3750,7 @@
       <c r="L26" s="41"/>
       <c r="N26" s="46" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>,output</v>
       </c>
       <c r="O26" s="47" t="str">
         <f t="shared" si="2"/>
@@ -3770,13 +3759,13 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="55" t="str">
         <f>IF(C17&lt;&gt;"",$B$3&amp;C17&amp;$B$4&amp;E17&amp;$B$5,"")</f>
-        <v>&lt;input type='text' id='periods_hours'&gt;&lt;spam id='periods_hours_mssg'&gt;&lt;/spam&gt;</v>
+        <v>&lt;input type='text' id='junks_task'&gt;&lt;spam id='junks_task_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
@@ -3785,7 +3774,7 @@
       <c r="G30" s="32"/>
       <c r="H30" s="55" t="str">
         <f>IF(I17&lt;&gt;"",$B$3&amp;I17&amp;$B$4&amp;K17&amp;$B$5,"")</f>
-        <v/>
+        <v>&lt;input type='text' id='junks_comments'&gt;&lt;spam id='junks_comments_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -3796,7 +3785,7 @@
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="55" t="str">
         <f t="shared" ref="B31:B39" si="4">IF(C18&lt;&gt;"",$B$3&amp;C18&amp;$B$4&amp;E18&amp;$B$5,"")</f>
-        <v>&lt;input type='text' id='periods_minutes'&gt;&lt;spam id='periods_minutes_mssg'&gt;&lt;/spam&gt;</v>
+        <v>&lt;input type='text' id='junks_project'&gt;&lt;spam id='junks_project_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
@@ -3816,7 +3805,7 @@
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="55" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;input type='text' id='periods_seconds'&gt;&lt;spam id='periods_seconds_mssg'&gt;&lt;/spam&gt;</v>
+        <v>&lt;input type='text' id='junks_stage'&gt;&lt;spam id='junks_stage_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
@@ -3836,7 +3825,7 @@
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_parent'&gt;&lt;spam id='junks_parent_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
@@ -3856,7 +3845,7 @@
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_score'&gt;&lt;spam id='junks_score_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
@@ -3876,7 +3865,7 @@
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_creator'&gt;&lt;spam id='junks_creator_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C35" s="32"/>
       <c r="D35" s="32"/>
@@ -3896,7 +3885,7 @@
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_adopter'&gt;&lt;spam id='junks_adopter_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
@@ -3916,7 +3905,7 @@
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_evidence'&gt;&lt;spam id='junks_evidence_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C37" s="32"/>
       <c r="D37" s="32"/>
@@ -3936,7 +3925,7 @@
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_reason'&gt;&lt;spam id='junks_reason_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C38" s="32"/>
       <c r="D38" s="32"/>
@@ -3956,7 +3945,7 @@
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="55" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>&lt;input type='text' id='junks_output'&gt;&lt;spam id='junks_output_mssg'&gt;&lt;/spam&gt;</v>
       </c>
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
@@ -3975,7 +3964,7 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="57" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C41" s="57"/>
       <c r="D41" s="57"/>
@@ -3983,12 +3972,12 @@
       <c r="F41" s="57"/>
       <c r="G41" s="57"/>
       <c r="H41" s="10" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="57" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C42" s="57"/>
       <c r="D42" s="57"/>
@@ -3998,7 +3987,7 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="57" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C43" s="57"/>
       <c r="D43" s="57"/>
@@ -4008,12 +3997,12 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D46" s="10" t="str">
         <f>'AutoLaravel v1'!D67&amp;'AutoLaravel v1'!D66</f>
@@ -4026,7 +4015,7 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D47" s="10" t="str">
         <f>'AutoLaravel v1'!D67</f>
@@ -4036,7 +4025,7 @@
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D48" s="10" t="str">
         <f>'AutoLaravel v1'!D68</f>
@@ -4049,7 +4038,7 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D49" s="10" t="str">
         <f>D46&amp;"_submit"</f>
@@ -4066,7 +4055,7 @@
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D50" s="32" t="str">
         <f>D47&amp;"/"&amp;D46</f>
@@ -4075,7 +4064,7 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -4086,7 +4075,7 @@
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="55" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
@@ -4096,7 +4085,7 @@
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="55" t="str">
         <f>IF(B17="","",$A$2&amp;B17&amp;$A$3&amp;C17&amp;$A$4)&amp;IF(B18="","",$A$2&amp;B18&amp;$A$3&amp;C18&amp;$A$4)</f>
-        <v>var hours=$('#periods_hours').val();var minutes=$('#periods_minutes').val();</v>
+        <v>var task=$('#junks_task').val();var project=$('#junks_project').val();</v>
       </c>
       <c r="C54" s="32"/>
       <c r="D54" s="32"/>
@@ -4106,7 +4095,7 @@
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="str">
         <f>IF(B19="","",$A$2&amp;B19&amp;$A$3&amp;C19&amp;$A$4)&amp;IF(B20="","",$A$2&amp;B20&amp;$A$3&amp;C20&amp;$A$4)</f>
-        <v>var seconds=$('#periods_seconds').val();</v>
+        <v>var stage=$('#junks_stage').val();var parent=$('#junks_parent').val();</v>
       </c>
       <c r="C55" s="32"/>
       <c r="D55" s="32"/>
@@ -4116,7 +4105,7 @@
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="55" t="str">
         <f>IF(B21="","",$A$2&amp;B21&amp;$A$3&amp;B21&amp;$A$4)&amp;IF(B22="","",$A$2&amp;B22&amp;$A$3&amp;B22&amp;$A$4)</f>
-        <v/>
+        <v>var score=$('#score').val();var creator=$('#creator').val();</v>
       </c>
       <c r="C56" s="32"/>
       <c r="D56" s="32"/>
@@ -4126,7 +4115,7 @@
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="55" t="str">
         <f>IF(B23="","",$A$2&amp;B23&amp;$A$3&amp;B23&amp;$A$4)&amp;IF(B24="","",$A$2&amp;B24&amp;$A$3&amp;B24&amp;$A$4)</f>
-        <v/>
+        <v>var adopter=$('#adopter').val();var evidence=$('#evidence').val();</v>
       </c>
       <c r="C57" s="32"/>
       <c r="D57" s="32"/>
@@ -4136,7 +4125,7 @@
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="55" t="str">
         <f>IF(B25="","",$A$2&amp;B25&amp;$A$3&amp;B25&amp;$A$4)&amp;IF(B26="","",$A$2&amp;B26&amp;$A$3&amp;B26&amp;$A$4)</f>
-        <v/>
+        <v>var reason=$('#reason').val();var output=$('#output').val();</v>
       </c>
       <c r="C58" s="32"/>
       <c r="D58" s="32"/>
@@ -4146,7 +4135,7 @@
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="56" t="str">
         <f>IF(H17="","",$A$2&amp;H17&amp;$A$3&amp;H17&amp;$A$4)&amp;IF(H18="","",$A$2&amp;H18&amp;$A$3&amp;H18&amp;$A$4)</f>
-        <v/>
+        <v>var comments=$('#comments').val();</v>
       </c>
       <c r="C59" s="32"/>
       <c r="D59" s="32"/>
@@ -4195,31 +4184,31 @@
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" s="22" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="56" t="str">
         <f>N17&amp;IF(B17&lt;&gt;"",":","")&amp;B17&amp;N18&amp;IF(B18&lt;&gt;"",":","")&amp;B18&amp;N19&amp;IF(B19&lt;&gt;"",":","")&amp;B19&amp;N20&amp;IF(B20&lt;&gt;"",":","")&amp;B20</f>
-        <v>hours:hours,minutes:minutes,seconds:seconds</v>
+        <v>task:task,project:project,stage:stage,parent:parent</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="56" t="str">
         <f>N21&amp;IF(B21&lt;&gt;"",":","")&amp;B21&amp;N22&amp;IF(B22&lt;&gt;"",":","")&amp;B22&amp;N23&amp;IF(B23&lt;&gt;"",":","")&amp;B23&amp;N24&amp;IF(B24&lt;&gt;"",":","")&amp;B24</f>
-        <v/>
+        <v>,score:score,creator:creator,adopter:adopter,evidence:evidence</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="56" t="str">
         <f t="shared" ref="B67" si="6">N25&amp;IF(B25&lt;&gt;"",":","")&amp;B25&amp;N26&amp;IF(B26&lt;&gt;"",":","")&amp;B26</f>
-        <v/>
+        <v>,reason:reason,output:output</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="55" t="str">
         <f>O17&amp;IF(H17&lt;&gt;"",":","")&amp;H17&amp;O18&amp;IF(H18&lt;&gt;"",":","")&amp;H18&amp;O19&amp;IF(H19&lt;&gt;"",":","")&amp;H19&amp;O20&amp;IF(H20&lt;&gt;"",":","")&amp;H20</f>
-        <v/>
+        <v>,comments:comments</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
@@ -4236,7 +4225,7 @@
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
@@ -4247,12 +4236,12 @@
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="22" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
@@ -4266,16 +4255,16 @@
       <c r="E77" s="32"/>
       <c r="F77" s="32"/>
       <c r="G77" s="16" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="H77" s="16" t="str">
         <f>'AutoLaravel v1'!D45</f>
-        <v>periods</v>
+        <v>junks</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D78" s="58" t="str">
         <f>"public function post"&amp;E46&amp;"() {"</f>
@@ -4284,32 +4273,32 @@
       <c r="E78" s="32"/>
       <c r="F78" s="32"/>
       <c r="G78" s="16" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H78" s="16" t="str">
         <f>'AutoLaravel v1'!G45</f>
-        <v>Period</v>
+        <v>Junk</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D79" s="58" t="str">
         <f>"$"&amp;B17&amp;"=$_POST['"&amp;B17&amp;"'];"</f>
-        <v>$hours=$_POST['hours'];</v>
+        <v>$task=$_POST['task'];</v>
       </c>
       <c r="E79" s="32"/>
       <c r="F79" s="32"/>
       <c r="G79" s="16" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="H79" s="16" t="str">
         <f>"$"&amp;'AutoLaravel v1'!F45</f>
-        <v>$period</v>
+        <v>$junk</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D80" s="58" t="str">
         <f>"$"&amp;B18&amp;"=$_POST['"&amp;B18&amp;"'];"</f>
-        <v>$minutes=$_POST['minutes'];</v>
+        <v>$project=$_POST['project'];</v>
       </c>
       <c r="E80" s="32"/>
       <c r="F80" s="32"/>
@@ -4317,14 +4306,14 @@
     <row r="81" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D81" s="58" t="str">
         <f>"$"&amp;B19&amp;"=$_POST['"&amp;B19&amp;"'];"</f>
-        <v>$seconds=$_POST['seconds'];</v>
+        <v>$stage=$_POST['stage'];</v>
       </c>
       <c r="E81" s="32"/>
       <c r="F81" s="32"/>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D82" s="58" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E82" s="32"/>
       <c r="F82" s="32"/>
@@ -4332,7 +4321,7 @@
     <row r="83" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D83" s="58" t="str">
         <f>H79&amp;"=New "&amp;H78&amp;";"</f>
-        <v>$period=New Period;</v>
+        <v>$junk=New Junk;</v>
       </c>
       <c r="E83" s="32"/>
       <c r="F83" s="32"/>
@@ -4340,7 +4329,7 @@
     <row r="84" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D84" s="55" t="str">
         <f>IF(B17&lt;&gt;"",$H$79&amp;$C$2&amp;B17&amp;"=$"&amp;B17&amp;";","")</f>
-        <v>$period-&gt;hours=$hours;</v>
+        <v>$junk-&gt;task=$task;</v>
       </c>
       <c r="E84" s="32"/>
       <c r="F84" s="32"/>
@@ -4348,7 +4337,7 @@
     <row r="85" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D85" s="55" t="str">
         <f t="shared" ref="D85:D93" si="8">IF(B18&lt;&gt;"",$H$79&amp;$C$2&amp;B18&amp;"=$"&amp;B18&amp;";","")</f>
-        <v>$period-&gt;minutes=$minutes;</v>
+        <v>$junk-&gt;project=$project;</v>
       </c>
       <c r="E85" s="32"/>
       <c r="F85" s="32"/>
@@ -4356,7 +4345,7 @@
     <row r="86" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D86" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>$period-&gt;seconds=$seconds;</v>
+        <v>$junk-&gt;stage=$stage;</v>
       </c>
       <c r="E86" s="32"/>
       <c r="F86" s="32"/>
@@ -4364,7 +4353,7 @@
     <row r="87" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D87" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;parent=$parent;</v>
       </c>
       <c r="E87" s="32"/>
       <c r="F87" s="32"/>
@@ -4372,7 +4361,7 @@
     <row r="88" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D88" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;score=$score;</v>
       </c>
       <c r="E88" s="32"/>
       <c r="F88" s="32"/>
@@ -4380,7 +4369,7 @@
     <row r="89" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D89" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;creator=$creator;</v>
       </c>
       <c r="E89" s="32"/>
       <c r="F89" s="32"/>
@@ -4388,7 +4377,7 @@
     <row r="90" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D90" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;adopter=$adopter;</v>
       </c>
       <c r="E90" s="32"/>
       <c r="F90" s="32"/>
@@ -4396,7 +4385,7 @@
     <row r="91" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D91" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;evidence=$evidence;</v>
       </c>
       <c r="E91" s="32"/>
       <c r="F91" s="32"/>
@@ -4404,7 +4393,7 @@
     <row r="92" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D92" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;reason=$reason;</v>
       </c>
       <c r="E92" s="32"/>
       <c r="F92" s="32"/>
@@ -4412,14 +4401,14 @@
     <row r="93" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D93" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>$junk-&gt;output=$output;</v>
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="32"/>
     </row>
     <row r="94" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D94" s="58" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E94" s="32"/>
       <c r="F94" s="32"/>
@@ -4427,14 +4416,14 @@
     <row r="95" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D95" s="58" t="str">
         <f>H79&amp;C2&amp;"save();"</f>
-        <v>$period-&gt;save();</v>
+        <v>$junk-&gt;save();</v>
       </c>
       <c r="E95" s="32"/>
       <c r="F95" s="32"/>
     </row>
     <row r="96" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D96" s="58" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E96" s="32"/>
       <c r="F96" s="32"/>
@@ -4456,10 +4445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2700" activePane="bottomLeft"/>
-      <selection activeCell="C3" sqref="C3"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72:D74"/>
+    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4469,55 +4456,68 @@
     <col min="8" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>162</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>163</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>146</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="18" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="str">
+        <f>"_table --fields="</f>
+        <v>_table --fields=</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>128</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>411</v>
+        <v>403</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4543,7 +4543,7 @@
         <v>161</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D13" s="9"/>
     </row>
@@ -4552,7 +4552,7 @@
         <v>126</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -4703,7 +4703,7 @@
         <v>93</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D40" s="9"/>
       <c r="F40" s="10" t="s">
@@ -4738,7 +4738,7 @@
       </c>
       <c r="M42" s="16" t="str">
         <f>IF(SUM(J47:K56)&gt;0,B2&amp;P56&amp;Q56&amp;B3,"")</f>
-        <v>--fields="hours:string,minutes:string,seconds:integer"</v>
+        <v>--fields="task:string,project:string,stage:string,parent:string,score:integer,creator:string,adopter:string,evidence:string,reason:string,output:string,comments:string"</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
@@ -4751,15 +4751,15 @@
         <v>102</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>414</v>
+        <v>460</v>
       </c>
       <c r="F45" s="16" t="str">
         <f>LEFT(D45,LEN(D45)-1)</f>
-        <v>period</v>
+        <v>junk</v>
       </c>
       <c r="G45" s="16" t="str">
         <f>UPPER(LEFT(F45,1))&amp;RIGHT(F45,LEN(F45)-1)</f>
-        <v>Period</v>
+        <v>Junk</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>103</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>415</v>
+        <v>461</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>134</v>
@@ -4799,34 +4799,38 @@
       <c r="F47" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
+      <c r="G47" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="J47" s="16">
         <f>IF(C47="",0,1)</f>
         <v>1</v>
       </c>
       <c r="K47" s="16">
         <f>IF(G47="",0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="16" t="s">
         <v>133</v>
       </c>
       <c r="N47" s="16" t="str">
         <f>IF(AND(C47&lt;&gt;"",D47&lt;&gt;""),IF(N46="concatenator1","",",")&amp;C47&amp;":"&amp;D47,"")</f>
-        <v>hours:string</v>
+        <v>task:string</v>
       </c>
       <c r="O47" s="16" t="str">
         <f>IF(AND(G47&lt;&gt;"",H47&lt;&gt;""),","&amp;G47&amp;":"&amp;H47,"")</f>
-        <v/>
+        <v>,comments:string</v>
       </c>
       <c r="P47" s="16" t="str">
         <f>P46&amp;N47</f>
-        <v>hours:string</v>
+        <v>task:string</v>
       </c>
       <c r="Q47" s="16" t="str">
         <f>Q46&amp;O47</f>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
@@ -4834,7 +4838,7 @@
         <v>104</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>416</v>
+        <v>462</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>134</v>
@@ -4857,7 +4861,7 @@
       </c>
       <c r="N48" s="16" t="str">
         <f t="shared" ref="N48:N56" si="2">IF(AND(C48&lt;&gt;"",D48&lt;&gt;""),IF(N47="concatenator1","",",")&amp;C48&amp;":"&amp;D48,"")</f>
-        <v>,minutes:string</v>
+        <v>,project:string</v>
       </c>
       <c r="O48" s="16" t="str">
         <f t="shared" ref="O48:O56" si="3">IF(AND(G48&lt;&gt;"",H48&lt;&gt;""),","&amp;G48&amp;":"&amp;H48,"")</f>
@@ -4865,11 +4869,11 @@
       </c>
       <c r="P48" s="16" t="str">
         <f t="shared" ref="P48:P56" si="4">P47&amp;N48</f>
-        <v>hours:string,minutes:string</v>
+        <v>task:string,project:string</v>
       </c>
       <c r="Q48" s="16" t="str">
         <f t="shared" ref="Q48:Q56" si="5">Q47&amp;O48</f>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.25">
@@ -4877,10 +4881,10 @@
         <v>105</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>417</v>
+        <v>463</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>115</v>
@@ -4900,7 +4904,7 @@
       </c>
       <c r="N49" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>,seconds:integer</v>
+        <v>,stage:string</v>
       </c>
       <c r="O49" s="16" t="str">
         <f t="shared" si="3"/>
@@ -4908,19 +4912,23 @@
       </c>
       <c r="P49" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string</v>
       </c>
       <c r="Q49" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
+      <c r="C50" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F50" s="10" t="s">
         <v>116</v>
       </c>
@@ -4928,7 +4936,7 @@
       <c r="H50" s="9"/>
       <c r="J50" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" s="16">
         <f t="shared" si="1"/>
@@ -4939,7 +4947,7 @@
       </c>
       <c r="N50" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,parent:string</v>
       </c>
       <c r="O50" s="16" t="str">
         <f t="shared" si="3"/>
@@ -4947,19 +4955,23 @@
       </c>
       <c r="P50" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string</v>
       </c>
       <c r="Q50" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
+      <c r="C51" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>133</v>
+      </c>
       <c r="F51" s="10" t="s">
         <v>117</v>
       </c>
@@ -4967,7 +4979,7 @@
       <c r="H51" s="9"/>
       <c r="J51" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" s="16">
         <f t="shared" si="1"/>
@@ -4978,7 +4990,7 @@
       </c>
       <c r="N51" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,score:integer</v>
       </c>
       <c r="O51" s="16" t="str">
         <f t="shared" si="3"/>
@@ -4986,19 +4998,23 @@
       </c>
       <c r="P51" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string,score:integer</v>
       </c>
       <c r="Q51" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+      <c r="C52" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F52" s="10" t="s">
         <v>118</v>
       </c>
@@ -5006,7 +5022,7 @@
       <c r="H52" s="9"/>
       <c r="J52" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="16">
         <f t="shared" si="1"/>
@@ -5017,7 +5033,7 @@
       </c>
       <c r="N52" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,creator:string</v>
       </c>
       <c r="O52" s="16" t="str">
         <f t="shared" si="3"/>
@@ -5025,19 +5041,23 @@
       </c>
       <c r="P52" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string,score:integer,creator:string</v>
       </c>
       <c r="Q52" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
+      <c r="C53" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F53" s="10" t="s">
         <v>119</v>
       </c>
@@ -5045,7 +5065,7 @@
       <c r="H53" s="9"/>
       <c r="J53" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="16">
         <f t="shared" si="1"/>
@@ -5056,7 +5076,7 @@
       </c>
       <c r="N53" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,adopter:string</v>
       </c>
       <c r="O53" s="16" t="str">
         <f t="shared" si="3"/>
@@ -5064,19 +5084,23 @@
       </c>
       <c r="P53" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string,score:integer,creator:string,adopter:string</v>
       </c>
       <c r="Q53" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
+      <c r="C54" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F54" s="10" t="s">
         <v>120</v>
       </c>
@@ -5084,7 +5108,7 @@
       <c r="H54" s="9"/>
       <c r="J54" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" s="16">
         <f t="shared" si="1"/>
@@ -5095,7 +5119,7 @@
       </c>
       <c r="N54" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,evidence:string</v>
       </c>
       <c r="O54" s="16" t="str">
         <f t="shared" si="3"/>
@@ -5103,19 +5127,23 @@
       </c>
       <c r="P54" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string,score:integer,creator:string,adopter:string,evidence:string</v>
       </c>
       <c r="Q54" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
+      <c r="C55" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F55" s="10" t="s">
         <v>121</v>
       </c>
@@ -5123,7 +5151,7 @@
       <c r="H55" s="9"/>
       <c r="J55" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" s="16">
         <f t="shared" si="1"/>
@@ -5134,7 +5162,7 @@
       </c>
       <c r="N55" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,reason:string</v>
       </c>
       <c r="O55" s="16" t="str">
         <f t="shared" si="3"/>
@@ -5142,19 +5170,23 @@
       </c>
       <c r="P55" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string,score:integer,creator:string,adopter:string,evidence:string,reason:string</v>
       </c>
       <c r="Q55" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
+      <c r="C56" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="F56" s="10" t="s">
         <v>122</v>
       </c>
@@ -5162,7 +5194,7 @@
       <c r="H56" s="9"/>
       <c r="J56" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" s="16">
         <f t="shared" si="1"/>
@@ -5173,7 +5205,7 @@
       </c>
       <c r="N56" s="16" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>,output:string</v>
       </c>
       <c r="O56" s="16" t="str">
         <f t="shared" si="3"/>
@@ -5181,11 +5213,11 @@
       </c>
       <c r="P56" s="16" t="str">
         <f t="shared" si="4"/>
-        <v>hours:string,minutes:string,seconds:integer</v>
+        <v>task:string,project:string,stage:string,parent:string,score:integer,creator:string,adopter:string,evidence:string,reason:string,output:string</v>
       </c>
       <c r="Q56" s="16" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>,comments:string</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
@@ -5199,7 +5231,7 @@
       </c>
       <c r="C60" s="23" t="str">
         <f>A4&amp;A5&amp;A6&amp;D45&amp;B1&amp;M42</f>
-        <v>php artisan generate:migration create_periods_table --fields="hours:string,minutes:string,seconds:integer"</v>
+        <v>php artisan generate:migration create_junks_table --fields="task:string,project:string,stage:string,parent:string,score:integer,creator:string,adopter:string,evidence:string,reason:string,output:string,comments:string"</v>
       </c>
       <c r="D60" s="23"/>
       <c r="E60" s="23"/>
@@ -5224,7 +5256,7 @@
       </c>
       <c r="C62" s="23" t="str">
         <f>A4&amp;B4&amp;G45</f>
-        <v>php artisan generate:model Period</v>
+        <v>php artisan generate:model Junk</v>
       </c>
       <c r="D62" s="23"/>
       <c r="E62" s="23"/>
@@ -5244,7 +5276,7 @@
         <v>149</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F66" s="20" t="s">
         <v>184</v>
@@ -5260,7 +5292,7 @@
         <v>150</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="F67" s="20" t="s">
         <v>183</v>
@@ -5275,7 +5307,7 @@
         <v>155</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="F68" s="24" t="s">
         <v>156</v>
@@ -5346,7 +5378,7 @@
         <v>160</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
@@ -5362,7 +5394,7 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="10" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
@@ -5377,7 +5409,7 @@
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
@@ -5385,34 +5417,32 @@
         <v>189</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>380</v>
+        <v>460</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" s="10" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>381</v>
+        <v>470</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D85" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C86" s="23" t="s">
-        <v>382</v>
+      <c r="C86" s="23" t="str">
+        <f>C3&amp;D84&amp;C4&amp;D83&amp;C5&amp;C6&amp;D84&amp;":"&amp;D85&amp;C6</f>
+        <v>php artisan generate:migration add_notice_to_junks_table --fields="notice:integer"</v>
       </c>
       <c r="D86" s="23"/>
       <c r="E86" s="23"/>
@@ -5424,7 +5454,7 @@
       <c r="K86" s="23"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D47:D56 H47:H56">
       <formula1>$M$47:$M$56</formula1>
     </dataValidation>
@@ -5438,7 +5468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5540,53 +5572,53 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D23" s="22"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C25" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -5596,7 +5628,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -5616,7 +5648,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F36" s="29"/>
     </row>
@@ -5636,7 +5668,7 @@
   <dimension ref="B3:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C20"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,9 +5766,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I53"/>
+  <dimension ref="B2:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5844,33 +5878,33 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="10" t="s">
-        <v>226</v>
+      <c r="C27" s="22" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C28" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C29" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C30" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C31" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C32" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -5881,96 +5915,107 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C37" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C38" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C40" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C41" s="27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C42" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>238</v>
+        <v>457</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
-        <v>240</v>
+      <c r="C45" s="22" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="10" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="10" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5978,8 +6023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5991,92 +6036,92 @@
   <sheetData>
     <row r="1" spans="1:10" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>263</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>265</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D11" s="22" t="str">
         <f>A1&amp;D7&amp;A2&amp;D9&amp;A3</f>
-        <v>Route::('alejo','alex');</v>
+        <v>Route::('task','taskController');</v>
       </c>
       <c r="E11" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="31" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="31" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H14" s="31"/>
       <c r="I14" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D15" s="22" t="str">
         <f>$B$1&amp;B15&amp;UPPER(LEFT(C15,1))&amp;RIGHT(C15,LEN(C15)-1)&amp;$B$2</f>
@@ -6084,19 +6129,19 @@
       </c>
       <c r="G15" s="11" t="str">
         <f>$D$7&amp;"/"&amp;C15</f>
-        <v>alejo/addtask</v>
+        <v>task/addtask</v>
       </c>
       <c r="I15" s="22" t="str">
         <f>$B$3&amp;G15&amp;$C$1&amp;C15&amp;$C$2</f>
-        <v>{{link_to('alejo/addtask','addtask'}}</v>
+        <v>{{link_to('task/addtask','addtask'}}</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D16" s="22" t="str">
         <f>$B$1&amp;B16&amp;UPPER(LEFT(C16,1))&amp;RIGHT(C16,LEN(C16)-1)&amp;$B$2</f>
@@ -6104,10 +6149,10 @@
       </c>
       <c r="G16" s="11" t="str">
         <f>$D$7&amp;"/"&amp;C16</f>
-        <v>alejo/addtask</v>
+        <v>task/addtask</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -6119,8 +6164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6130,142 +6175,142 @@
   <sheetData>
     <row r="1" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="F2" s="48" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="G2" s="48" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E3" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>440</v>
+      </c>
+      <c r="G3" s="49" t="s">
         <v>448</v>
-      </c>
-      <c r="F3" s="49" t="s">
-        <v>451</v>
-      </c>
-      <c r="G3" s="49" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="F4" s="49" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="48" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="53" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
@@ -6275,7 +6320,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="53" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="53"/>
@@ -6285,22 +6330,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="16" t="str">
@@ -6310,18 +6355,18 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C21" s="9"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="50" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
@@ -6338,7 +6383,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="50" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -6355,7 +6400,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="51" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
@@ -6377,28 +6422,28 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="G33" s="16" t="s">
         <v>327</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="16" t="str">
@@ -6412,10 +6457,10 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="16"/>
@@ -6423,10 +6468,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="16" t="str">
@@ -6440,7 +6485,7 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>167</v>
@@ -6451,34 +6496,34 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D42" s="22" t="str">
         <f>F34&amp;"_id"</f>
         <v>project_id</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -6506,7 +6551,7 @@
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -6534,25 +6579,25 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" s="22" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D59" s="22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -6561,7 +6606,7 @@
         <v>$project=Project::all();</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -6570,7 +6615,7 @@
         <v>foreach ($project as $value){</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -6579,7 +6624,7 @@
         <v xml:space="preserve">     $row=Project::find($value-&gt;id);</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -6588,7 +6633,7 @@
         <v xml:space="preserve">     $owner=$value-&gt;p_owner;</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -6597,22 +6642,22 @@
         <v xml:space="preserve">     $allowed=$row-&gt;thetask;</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D65" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D67" s="22" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
@@ -6623,108 +6668,108 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D69" s="10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D70" s="10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D71" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D72" s="10" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D73" s="10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D74" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D75" s="22" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D76" s="22" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D77" s="10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D78" s="10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D79" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D80" s="10" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D81" s="10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D82" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D84" s="22" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D85" s="22" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E95" s="16" t="str">
         <f>LEFT(C95,LEN(C95)-1)</f>
@@ -6737,10 +6782,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E96" s="16" t="str">
         <f>LEFT(C96,LEN(C96)-1)</f>
@@ -6753,33 +6798,33 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="16"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="16"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -6796,12 +6841,12 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B104" s="27" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="59" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="59"/>
@@ -6814,7 +6859,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="59" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="59"/>
@@ -6827,18 +6872,18 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F109" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="D110" s="52" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E110" s="52"/>
       <c r="F110" s="16" t="str">
@@ -6852,10 +6897,10 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="D111" s="52" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="E111" s="52"/>
       <c r="F111" s="16"/>
@@ -6863,10 +6908,10 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="D112" s="52" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E112" s="52"/>
       <c r="F112" s="16" t="str">
@@ -6880,10 +6925,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="D113" s="52" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E113" s="52"/>
       <c r="F113" s="16"/>
@@ -6891,10 +6936,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="D114" s="52" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="E114" s="52"/>
       <c r="F114" s="16" t="str">
@@ -6908,7 +6953,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="D115" s="52" t="s">
         <v>167</v>
@@ -6919,10 +6964,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="D116" s="52" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E116" s="52"/>
       <c r="F116" s="16"/>
@@ -6930,10 +6975,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="D117" s="52" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="E117" s="52"/>
       <c r="F117" s="16"/>
@@ -6941,10 +6986,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="D118" s="52" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="E118" s="52"/>
       <c r="F118" s="16"/>
@@ -6952,7 +6997,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -6966,7 +7011,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -6977,7 +7022,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B126" s="22" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -7012,7 +7057,7 @@
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="22" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
@@ -7027,12 +7072,12 @@
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="22" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="22" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
@@ -7061,12 +7106,12 @@
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="22" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="22" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
@@ -7086,7 +7131,7 @@
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="27" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>